<commit_message>
Added run result and script
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/Run results and used files.xlsx
+++ b/Results and scripts_mp/Run results and used files.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Input filename</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>ajo päättyi 12:16</t>
+  </si>
+  <si>
+    <t>11062013_20d_Cvap_Dillon</t>
+  </si>
+  <si>
+    <t>ajo aloitettu 16:18</t>
+  </si>
+  <si>
+    <t>run_20130612T042435</t>
   </si>
 </sst>
 </file>
@@ -445,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F12"/>
+  <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,8 +647,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10.6</v>
+      <c r="A12" s="1">
+        <v>41435</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -652,6 +661,20 @@
       </c>
       <c r="E12" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>41436</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added validation scripts and test run data
</commit_message>
<xml_diff>
--- a/Results and scripts_mp/Run results and used files.xlsx
+++ b/Results and scripts_mp/Run results and used files.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Input filename</t>
   </si>
@@ -115,6 +115,21 @@
   </si>
   <si>
     <t>run_20130612T042435</t>
+  </si>
+  <si>
+    <t>run_20130613T132541</t>
+  </si>
+  <si>
+    <t>12062013_validation_10sect</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>run_20130613T133513</t>
+  </si>
+  <si>
+    <t>13062013_validation_10_sect_test</t>
   </si>
 </sst>
 </file>
@@ -150,9 +165,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F13"/>
+  <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,8 +693,34 @@
         <v>31</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>41438</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>41438</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>